<commit_message>
update transit time final air traffic delay
</commit_message>
<xml_diff>
--- a/data/atfm_delay.xlsx
+++ b/data/atfm_delay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oburdash\dev\repos\standard_inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68CC84A7-3E6B-4041-97A4-E47458D5B18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5CF1048-C668-490B-A34F-1E1B551101AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -86,7 +86,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -158,34 +158,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -266,34 +266,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2012</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -525,7 +525,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="accent5">
                         <a:lumMod val="50000"/>
@@ -537,7 +537,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" b="1"/>
+                  <a:rPr lang="en-GB" sz="1400" b="1"/>
                   <a:t>Average delay per flight (minutes)</a:t>
                 </a:r>
               </a:p>
@@ -547,8 +547,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="5.461165048543689E-2"/>
-              <c:y val="0.1034082924508386"/>
+              <c:x val="4.1927731443756174E-2"/>
+              <c:y val="0.17949011723035332"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -564,7 +564,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="accent5">
                       <a:lumMod val="50000"/>
@@ -595,7 +595,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="accent5">
                     <a:lumMod val="50000"/>
@@ -627,7 +627,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="accent5">
                         <a:lumMod val="50000"/>
@@ -639,7 +639,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" b="1"/>
+                  <a:rPr lang="en-GB" sz="1400" b="1"/>
                   <a:t>Average traffic</a:t>
                 </a:r>
               </a:p>
@@ -658,7 +658,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="accent5">
                       <a:lumMod val="50000"/>
@@ -689,7 +689,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="accent5">
                     <a:lumMod val="50000"/>
@@ -718,6 +718,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="635546015"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -741,7 +742,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="accent5">
                     <a:lumMod val="50000"/>
@@ -1357,15 +1358,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
+      <xdr:colOff>426719</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>163830</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1659,16 +1660,16 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1682,9 +1683,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2021</v>
+        <v>2012</v>
       </c>
       <c r="B2">
         <v>0.48</v>
@@ -1696,9 +1697,9 @@
         <v>26427</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="B3">
         <v>0.39</v>
@@ -1710,9 +1711,9 @@
         <v>26215</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B4">
         <v>0.42</v>
@@ -1724,9 +1725,9 @@
         <v>26685</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="B5">
         <v>0.69</v>
@@ -1738,9 +1739,9 @@
         <v>27094</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B6">
         <v>0.67</v>
@@ -1752,9 +1753,9 @@
         <v>27844</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B7">
         <v>0.62</v>
@@ -1766,9 +1767,9 @@
         <v>29057</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="B8" s="2">
         <v>0.6</v>
@@ -1780,9 +1781,9 @@
         <v>30166</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="B9" s="2">
         <v>0.6</v>
@@ -1794,9 +1795,9 @@
         <v>30427</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="B10" s="2">
         <v>0.2</v>
@@ -1808,9 +1809,9 @@
         <v>13620</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2012</v>
+        <v>2021</v>
       </c>
       <c r="B11">
         <v>0.18</v>

</xml_diff>